<commit_message>
Updated credentials in Data sheet
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">TestCase</t>
   </si>
@@ -62,13 +62,16 @@
     <t xml:space="preserve">KoraV2AndroidTest</t>
   </si>
   <si>
-    <t xml:space="preserve">Jayakrishna.dandru@kore.com</t>
+    <t xml:space="preserve">hana@koraqa1.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Kore@123</t>
+    <t xml:space="preserve">kora@123</t>
   </si>
   <si>
     <t xml:space="preserve">KoraV2Web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">james@koraqa1.com</t>
   </si>
   <si>
     <t xml:space="preserve">s</t>
@@ -5391,7 +5394,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5430,7 +5433,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -5454,7 +5457,7 @@
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="12"/>
     </row>
@@ -8437,12 +8440,6 @@
       <c r="B1000" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Jayakrishna.dandru@kore.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="Kore@123"/>
-    <hyperlink ref="B3" r:id="rId3" display="Jayakrishna.dandru@kore.com"/>
-    <hyperlink ref="C3" r:id="rId4" display="Kore@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Modified credentials to O365 Modified properties file to maintain saperate testdata for o365 added other test cases in one to one Initiated Driver setup code change to copy Extent report file to other directory
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">ka6MtV8cwBHY </t>
   </si>
   <si>
-    <t xml:space="preserve">KoraV2AndroidTest</t>
+    <t xml:space="preserve">KoraV2hana</t>
   </si>
   <si>
     <t xml:space="preserve">hana@koraqa1.com</t>
@@ -5394,7 +5394,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added host and recepient usenames
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">kora@123</t>
   </si>
   <si>
-    <t xml:space="preserve">KoraV2Web</t>
+    <t xml:space="preserve">KoraV2james</t>
   </si>
   <si>
     <t xml:space="preserve">james@koraqa1.com</t>
@@ -5394,7 +5394,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>